<commit_message>
zile suspendare - needs checking
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/NotaContabila.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/NotaContabila.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C146B0-C61E-4889-9AD5-5EC2BE79371C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7812"/>
+    <workbookView xWindow="1656" yWindow="948" windowWidth="23580" windowHeight="14304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>Nota de contabilitate</t>
   </si>
@@ -102,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
@@ -257,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -285,18 +291,11 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -315,24 +314,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -340,11 +321,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="4" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -618,21 +611,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L29" sqref="L29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -645,55 +638,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="32" t="s">
+      <c r="A5" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="32"/>
-      <c r="C5" s="32"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -711,23 +704,23 @@
     <row r="7" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -781,11 +774,11 @@
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
@@ -800,28 +793,26 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="20"/>
       <c r="D15" s="4">
         <v>6458</v>
       </c>
       <c r="E15" s="4">
         <v>423</v>
       </c>
-      <c r="F15" s="10">
-        <v>2515</v>
-      </c>
+      <c r="F15" s="10"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="A16" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="22"/>
-      <c r="C16" s="23"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="20"/>
       <c r="D16" s="4">
         <v>641</v>
       </c>
@@ -841,7 +832,7 @@
       <c r="E17" s="27"/>
       <c r="F17" s="11">
         <f>SUM(F15:F16)</f>
-        <v>2515</v>
+        <v>0</v>
       </c>
       <c r="G17" s="2"/>
     </row>
@@ -864,22 +855,22 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="A20" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="20"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="17"/>
       <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
@@ -894,11 +885,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+      <c r="A22" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="30"/>
       <c r="D22" s="4">
         <v>421</v>
       </c>
@@ -909,11 +900,11 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+      <c r="A23" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="30"/>
+      <c r="C23" s="30"/>
       <c r="D23" s="4">
         <v>421</v>
       </c>
@@ -924,11 +915,11 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="4">
         <v>423</v>
       </c>
@@ -937,16 +928,16 @@
       </c>
       <c r="F24" s="8">
         <f>ROUND(F15*0.25, 0)</f>
-        <v>629</v>
+        <v>0</v>
       </c>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
+      <c r="A25" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="4">
         <v>421</v>
       </c>
@@ -957,11 +948,11 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
+      <c r="A26" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="4">
         <v>421</v>
       </c>
@@ -972,11 +963,11 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
       <c r="D27" s="4">
         <v>423</v>
       </c>
@@ -985,7 +976,7 @@
       </c>
       <c r="F27" s="8">
         <f>ROUND(F15*0.65*0.1,0)</f>
-        <v>163</v>
+        <v>0</v>
       </c>
       <c r="G27" s="5"/>
     </row>
@@ -999,7 +990,7 @@
       <c r="E28" s="27"/>
       <c r="F28" s="9">
         <f>SUM(F22:F27)</f>
-        <v>792</v>
+        <v>0</v>
       </c>
       <c r="G28" s="6"/>
     </row>
@@ -1022,22 +1013,22 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="C31" s="17"/>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-      <c r="F31" s="17"/>
-      <c r="G31" s="17"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="18" t="s">
+      <c r="A32" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="19"/>
-      <c r="C32" s="20"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="17"/>
       <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
@@ -1052,11 +1043,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="24" t="s">
+      <c r="A33" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="24"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="30"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="5">
         <v>646</v>
       </c>
@@ -1081,22 +1072,22 @@
       <c r="G34" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+      <c r="A37" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="17"/>
-      <c r="C37" s="17"/>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17"/>
-      <c r="G37" s="17"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+      <c r="G37" s="29"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="20"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="17"/>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
@@ -1111,36 +1102,41 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="21" t="s">
+      <c r="A39" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23"/>
+      <c r="B39" s="19"/>
+      <c r="C39" s="20"/>
       <c r="D39" s="5">
         <v>635</v>
       </c>
       <c r="E39" s="5">
         <v>436</v>
       </c>
-      <c r="F39" s="34"/>
+      <c r="F39" s="13"/>
       <c r="G39" s="5"/>
-    </row>
-    <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B40" s="14"/>
-      <c r="C40" s="14"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="35">
-        <f>F39</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:E34"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
@@ -1150,25 +1146,6 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="C8:F8"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:E34"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
rotunjire la 2 zecimale
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/NotaContabila.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/NotaContabila.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C146B0-C61E-4889-9AD5-5EC2BE79371C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1656" yWindow="948" windowWidth="23580" windowHeight="14304" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1656" yWindow="948" windowWidth="23256" windowHeight="13176"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +102,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
   </numFmts>
@@ -263,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -291,53 +285,50 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,21 +602,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -638,55 +629,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -704,23 +695,23 @@
     <row r="7" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -760,25 +751,25 @@
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="28"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="16"/>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
@@ -793,11 +784,11 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
       <c r="D15" s="4">
         <v>6458</v>
       </c>
@@ -808,11 +799,11 @@
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
       <c r="D16" s="4">
         <v>641</v>
       </c>
@@ -823,13 +814,13 @@
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="11">
         <f>SUM(F15:F16)</f>
         <v>0</v>
@@ -855,22 +846,22 @@
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="29"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29"/>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="A21" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="16"/>
-      <c r="C21" s="17"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="16"/>
       <c r="D21" s="3" t="s">
         <v>5</v>
       </c>
@@ -885,11 +876,11 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="4">
         <v>421</v>
       </c>
@@ -900,11 +891,11 @@
       <c r="G22" s="5"/>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="30" t="s">
+      <c r="A23" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="20"/>
       <c r="D23" s="4">
         <v>421</v>
       </c>
@@ -915,11 +906,11 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="30" t="s">
+      <c r="A24" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="20"/>
       <c r="D24" s="4">
         <v>423</v>
       </c>
@@ -933,11 +924,11 @@
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
       <c r="D25" s="4">
         <v>421</v>
       </c>
@@ -948,11 +939,11 @@
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
       <c r="D26" s="4">
         <v>421</v>
       </c>
@@ -963,11 +954,11 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="30" t="s">
+      <c r="A27" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
       <c r="D27" s="4">
         <v>423</v>
       </c>
@@ -981,13 +972,13 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+      <c r="A28" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="23"/>
       <c r="F28" s="9">
         <f>SUM(F22:F27)</f>
         <v>0</v>
@@ -1013,22 +1004,22 @@
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="13"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="16"/>
-      <c r="C32" s="17"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="16"/>
       <c r="D32" s="3" t="s">
         <v>5</v>
       </c>
@@ -1043,11 +1034,11 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
       <c r="D33" s="5">
         <v>646</v>
       </c>
@@ -1058,13 +1049,13 @@
       <c r="G33" s="5"/>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="25" t="s">
+      <c r="A34" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="27"/>
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="23"/>
       <c r="F34" s="12">
         <f>F33</f>
         <v>0</v>
@@ -1072,22 +1063,22 @@
       <c r="G34" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="29"/>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+      <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="16"/>
-      <c r="C38" s="17"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="16"/>
       <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
@@ -1102,41 +1093,22 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B39" s="19"/>
-      <c r="C39" s="20"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="5">
         <v>635</v>
       </c>
       <c r="E39" s="5">
         <v>436</v>
       </c>
-      <c r="F39" s="13"/>
+      <c r="F39" s="8"/>
       <c r="G39" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="A37:G37"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A32:C32"/>
-    <mergeCell ref="A31:G31"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:E34"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A22:C22"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A24:C24"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="A17:E17"/>
-    <mergeCell ref="A13:G13"/>
-    <mergeCell ref="A20:G20"/>
-    <mergeCell ref="A21:C21"/>
     <mergeCell ref="C7:F7"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A15:C15"/>
@@ -1146,6 +1118,25 @@
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="C8:F8"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="A13:G13"/>
+    <mergeCell ref="A20:G20"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A26:C26"/>
+    <mergeCell ref="A37:G37"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A32:C32"/>
+    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:E34"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
completeaza nota contabila please
</commit_message>
<xml_diff>
--- a/server/src/main/java/net/guides/springboot2/crud/templates/NotaContabila.xlsx
+++ b/server/src/main/java/net/guides/springboot2/crud/templates/NotaContabila.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexandru POP\Desktop\Proiecte\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\webapp-spring\server\src\main\java\net\guides\springboot2\crud\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EB2003-9791-48CC-B4D4-294AF30DFA22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1656" yWindow="948" windowWidth="23256" windowHeight="13176"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -110,10 +120,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="#,##0_ ;\-#,##0\ "/>
-  </numFmts>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
@@ -265,7 +272,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -284,18 +291,18 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -620,14 +627,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:J40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
@@ -635,63 +642,63 @@
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.28515625" customWidth="1"/>
+    <col min="6" max="6" width="17.28515625" style="15" customWidth="1"/>
     <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="F1" s="13"/>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="13"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
+      <c r="A3" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="28"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="13"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="F4" s="13"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="F5" s="13"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -700,29 +707,29 @@
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="13"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:10" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="32"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -731,7 +738,7 @@
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="F9" s="13"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -740,7 +747,7 @@
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="F10" s="13"/>
       <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -749,7 +756,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="13"/>
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -758,36 +765,36 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="F12" s="13"/>
       <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27"/>
+      <c r="D13" s="27"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
     <row r="14" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="16"/>
-      <c r="C14" s="17"/>
+      <c r="B14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G14" s="3" t="s">
@@ -795,59 +802,59 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="4">
         <v>6458</v>
       </c>
       <c r="E15" s="4">
         <v>423</v>
       </c>
-      <c r="F15" s="10"/>
+      <c r="F15" s="8"/>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="19"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="13">
+      <c r="B16" s="21"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="11">
         <v>4382</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E16" s="11">
         <v>423</v>
       </c>
-      <c r="F16" s="10"/>
-      <c r="G16" s="13"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="22"/>
       <c r="D17" s="4">
         <v>641</v>
       </c>
       <c r="E17" s="4">
         <v>421</v>
       </c>
-      <c r="F17" s="10"/>
+      <c r="F17" s="8"/>
       <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="11">
+      <c r="B18" s="25"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="9">
         <f>SUM(F15:F17)</f>
         <v>0</v>
       </c>
@@ -859,7 +866,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -868,33 +875,33 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="F20" s="13"/>
       <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="16"/>
-      <c r="C22" s="17"/>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
       <c r="D22" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G22" s="3" t="s">
@@ -902,11 +909,11 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B23" s="21"/>
-      <c r="C23" s="21"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
       <c r="D23" s="4">
         <v>421</v>
       </c>
@@ -917,44 +924,41 @@
       <c r="G23" s="5"/>
     </row>
     <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
+      <c r="A24" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
       <c r="D24" s="4">
         <v>421</v>
       </c>
       <c r="E24" s="4">
         <v>4315</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="12"/>
       <c r="G24" s="5"/>
     </row>
     <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
       <c r="D25" s="4">
         <v>423</v>
       </c>
       <c r="E25" s="4">
         <v>4315</v>
       </c>
-      <c r="F25" s="8">
-        <f>ROUND(F15*0.25, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="F25" s="8"/>
       <c r="G25" s="5"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
+      <c r="A26" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="21"/>
-      <c r="C26" s="21"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
       <c r="D26" s="4">
         <v>421</v>
       </c>
@@ -965,11 +969,11 @@
       <c r="G26" s="5"/>
     </row>
     <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="21"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
       <c r="D27" s="4">
         <v>421</v>
       </c>
@@ -980,31 +984,28 @@
       <c r="G27" s="5"/>
     </row>
     <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="B28" s="21"/>
-      <c r="C28" s="21"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
       <c r="D28" s="4">
         <v>423</v>
       </c>
       <c r="E28" s="4">
         <v>444</v>
       </c>
-      <c r="F28" s="8">
-        <f>ROUND(F15*0.65*0.1,0)</f>
-        <v>0</v>
-      </c>
+      <c r="F28" s="8"/>
       <c r="G28" s="5"/>
     </row>
     <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="24"/>
+      <c r="B29" s="25"/>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
       <c r="F29" s="9">
         <f>SUM(F23:F28)</f>
         <v>0</v>
@@ -1017,7 +1018,7 @@
       <c r="C30" s="7"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="F30" s="13"/>
       <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.25">
@@ -1026,33 +1027,33 @@
       <c r="C31" s="7"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="F31" s="13"/>
       <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B32" s="14"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="14"/>
-      <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
+      <c r="B32" s="16"/>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
     </row>
     <row r="33" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="19"/>
       <c r="D33" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G33" s="3" t="s">
@@ -1060,11 +1061,11 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A34" s="21" t="s">
+      <c r="A34" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="21"/>
-      <c r="C34" s="21"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
       <c r="D34" s="5">
         <v>646</v>
       </c>
@@ -1075,43 +1076,43 @@
       <c r="G34" s="5"/>
     </row>
     <row r="35" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A35" s="22" t="s">
+      <c r="A35" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
-      <c r="F35" s="12">
+      <c r="B35" s="25"/>
+      <c r="C35" s="25"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="26"/>
+      <c r="F35" s="10">
         <f>F34</f>
         <v>0</v>
       </c>
       <c r="G35" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="14"/>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="16"/>
     </row>
     <row r="39" spans="1:7" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="15" t="s">
+      <c r="A39" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
+      <c r="B39" s="18"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="14" t="s">
         <v>7</v>
       </c>
       <c r="G39" s="3" t="s">
@@ -1119,11 +1120,11 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="20"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="22"/>
       <c r="D40" s="5">
         <v>635</v>
       </c>

</xml_diff>